<commit_message>
Added Network Quote to Excel Folder
Added Network Quote to Excel Folder
</commit_message>
<xml_diff>
--- a/Excel/Network Equipment Quote.xlsx
+++ b/Excel/Network Equipment Quote.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\OneDrive\Documents\Tech\Git\Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\OneDrive\Documents\Tech\Git\Data_Analyst_Portfolio\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C5D4F7-D20F-4324-B426-D8AA0945F738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762246A6-C73C-47FA-8269-3EF3E0E5C71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Quote" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Price List'!$A$1:$E$49</definedName>
     <definedName name="Item_Code">'Price List'!$A$2:$A$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Customer Quote'!$B$1:$I$67</definedName>
     <definedName name="Quote">'Customer Quote'!$F$18</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -790,7 +791,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -831,7 +832,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -877,9 +877,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -889,21 +886,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="17" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -913,24 +910,23 @@
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -941,664 +937,7 @@
     <cellStyle name="Title" xfId="4" builtinId="15"/>
     <cellStyle name="Total" xfId="5" builtinId="25"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00;"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </right>
-        <top style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="3" tint="-0.249977111117893"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="27">
     <dxf>
       <font>
         <b val="0"/>
@@ -1695,6 +1034,74 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1747,6 +1154,574 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00;"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;\-&quot;$&quot;#,##0.00;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </right>
+        <top style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="3" tint="-0.249977111117893"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1767,25 +1742,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="B12:I44" totalsRowCount="1" headerRowDxfId="20" dataDxfId="18" totalsRowDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="B12:I44" totalsRowCount="1" headerRowDxfId="26" dataDxfId="25" totalsRowDxfId="24">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B13:I42">
     <sortCondition ref="C13"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="7" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Loc Code" dataDxfId="14" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Installation Location" dataDxfId="13" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Qty" dataDxfId="12" totalsRowDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Description" dataDxfId="11" totalsRowDxfId="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="23" totalsRowDxfId="22" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Loc Code" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Installation Location" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Qty" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Description" dataDxfId="15" totalsRowDxfId="14">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Category" dataDxfId="10" totalsRowDxfId="2">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Category" dataDxfId="13" totalsRowDxfId="12">
       <calculatedColumnFormula>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Retail Price" dataDxfId="9" totalsRowDxfId="1">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Retail Price" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Cost" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="0">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Cost" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8">
       <calculatedColumnFormula>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1794,14 +1769,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="parts" displayName="parts" ref="A1:E49" totalsRowShown="0" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="parts" displayName="parts" ref="A1:E49" totalsRowShown="0" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A1:E49" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Item Code" dataDxfId="26" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="6" xr3:uid="{2442E784-8D48-4B41-BF89-1D6895B5E246}" name="Manufacturer" dataDxfId="17" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="7" xr3:uid="{0303F34D-640B-440D-B851-A34A8F9338CB}" name="Category" dataDxfId="16" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Description" dataDxfId="25" dataCellStyle="Normal_Sheet1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Retail Price" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Item Code" dataDxfId="4" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="6" xr3:uid="{2442E784-8D48-4B41-BF89-1D6895B5E246}" name="Manufacturer" dataDxfId="3" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="7" xr3:uid="{0303F34D-640B-440D-B851-A34A8F9338CB}" name="Category" dataDxfId="2" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Description" dataDxfId="1" dataCellStyle="Normal_Sheet1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Retail Price" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2107,13 +2082,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J57"/>
+  <dimension ref="B1:J66"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="12" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomRight" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2134,37 +2109,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="26.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
       <c r="I1" s="17"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="42" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="17"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="55">
+      <c r="C3" s="53">
         <v>45119</v>
       </c>
       <c r="I3" s="17"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="43" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="18"/>
@@ -2185,1045 +2160,1084 @@
       <c r="I5" s="18"/>
     </row>
     <row r="6" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="41"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="21"/>
+      <c r="E7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="20"/>
       <c r="J7" s="13"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="21"/>
+      <c r="E8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="20"/>
       <c r="J8" s="13"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="39"/>
+      <c r="E9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="13"/>
     </row>
     <row r="10" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="47" t="s">
+      <c r="C10" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="26">
+      <c r="D10" s="24"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="25">
         <f>MATCH(Table2[[#Headers],[Description]],parts[#Headers],)</f>
         <v>4</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="25">
         <f>MATCH(Table2[[#Headers],[Category]],parts[#Headers],)</f>
         <v>3</v>
       </c>
-      <c r="H10" s="26">
+      <c r="H10" s="25">
         <f>MATCH(Table2[[#Headers],[Retail Price]],parts[#Headers],)</f>
         <v>5</v>
       </c>
-      <c r="I10" s="38"/>
+      <c r="I10" s="37"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="18"/>
-      <c r="C11" s="27"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="18"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="29"/>
-    </row>
-    <row r="12" spans="2:10" s="30" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="30" t="s">
+      <c r="E11" s="26"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="28"/>
+    </row>
+    <row r="12" spans="2:10" s="29" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="32" t="s">
+      <c r="H12" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="33" t="s">
+      <c r="I12" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="J12" s="34"/>
+      <c r="J12" s="33"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="62" t="s">
+      <c r="D13" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="E13" s="61">
+      <c r="E13" s="56">
         <v>1</v>
       </c>
-      <c r="F13" s="50" t="str">
+      <c r="F13" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>Cable Cove 2-Post Rack</v>
       </c>
-      <c r="G13" s="49" t="str">
+      <c r="G13" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Rack</v>
       </c>
-      <c r="H13" s="51">
+      <c r="H13" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>595</v>
       </c>
-      <c r="I13" s="52">
+      <c r="I13" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>595</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="60" t="s">
+      <c r="C14" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="62" t="s">
+      <c r="D14" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="E14" s="61">
+      <c r="E14" s="56">
         <v>1</v>
       </c>
-      <c r="F14" s="50" t="str">
+      <c r="F14" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>Cisco 2951, SRE 700 SM, NME WAE 502, WAAS Ent, IOS Sec PAK</v>
       </c>
-      <c r="G14" s="49" t="str">
+      <c r="G14" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Router</v>
       </c>
-      <c r="H14" s="51">
+      <c r="H14" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>14995</v>
       </c>
-      <c r="I14" s="52">
+      <c r="I14" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>14995</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="60" t="s">
+      <c r="C15" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="D15" s="62" t="s">
+      <c r="D15" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="E15" s="61">
+      <c r="E15" s="56">
         <v>6</v>
       </c>
-      <c r="F15" s="50" t="str">
+      <c r="F15" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>C9200-48T-E Catalyst 9200 Managed L3 Switch - 48 Ethernet Ports</v>
       </c>
-      <c r="G15" s="49" t="str">
+      <c r="G15" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Switch</v>
       </c>
-      <c r="H15" s="51">
+      <c r="H15" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>2665</v>
       </c>
-      <c r="I15" s="52">
+      <c r="I15" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>15990</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="D16" s="62" t="s">
+      <c r="D16" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="E16" s="61">
+      <c r="E16" s="56">
         <v>1</v>
       </c>
-      <c r="F16" s="50" t="str">
+      <c r="F16" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>19" Rounter Mount Kit</v>
       </c>
-      <c r="G16" s="49" t="str">
+      <c r="G16" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Mount Kit</v>
       </c>
-      <c r="H16" s="51">
+      <c r="H16" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>10</v>
       </c>
-      <c r="I16" s="52">
+      <c r="I16" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="D17" s="62" t="s">
+      <c r="D17" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="E17" s="61">
+      <c r="E17" s="56">
         <v>6</v>
       </c>
-      <c r="F17" s="50" t="str">
+      <c r="F17" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>19"  Switch Rack Mount Kit</v>
       </c>
-      <c r="G17" s="49" t="str">
+      <c r="G17" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Mount Kit</v>
       </c>
-      <c r="H17" s="51">
+      <c r="H17" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>10</v>
       </c>
-      <c r="I17" s="52">
+      <c r="I17" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>60</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="62" t="s">
+      <c r="D18" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="E18" s="61">
+      <c r="E18" s="56">
         <v>1</v>
       </c>
-      <c r="F18" s="50" t="str">
+      <c r="F18" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>Cable Cove 2-Post Rack</v>
       </c>
-      <c r="G18" s="49" t="str">
+      <c r="G18" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Rack</v>
       </c>
-      <c r="H18" s="51">
+      <c r="H18" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>595</v>
       </c>
-      <c r="I18" s="52">
+      <c r="I18" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>595</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="60" t="s">
+      <c r="C19" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="62" t="s">
+      <c r="D19" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="E19" s="61">
+      <c r="E19" s="56">
         <v>1</v>
       </c>
-      <c r="F19" s="50" t="str">
+      <c r="F19" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>Cisco 2951, SRE 700 SM, NME WAE 502, WAAS Ent, IOS Sec PAK</v>
       </c>
-      <c r="G19" s="49" t="str">
+      <c r="G19" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Router</v>
       </c>
-      <c r="H19" s="51">
+      <c r="H19" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>14995</v>
       </c>
-      <c r="I19" s="52">
+      <c r="I19" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>14995</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="D20" s="62" t="s">
+      <c r="D20" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="E20" s="61">
+      <c r="E20" s="56">
         <v>3</v>
       </c>
-      <c r="F20" s="50" t="str">
+      <c r="F20" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>C9200-48T-E Catalyst 9200 Managed L3 Switch - 48 Ethernet Ports</v>
       </c>
-      <c r="G20" s="49" t="str">
+      <c r="G20" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Switch</v>
       </c>
-      <c r="H20" s="51">
+      <c r="H20" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>2665</v>
       </c>
-      <c r="I20" s="52">
+      <c r="I20" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>7995</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="48" t="s">
+      <c r="B21" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="D21" s="62" t="s">
+      <c r="D21" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="61">
+      <c r="E21" s="56">
         <v>1</v>
       </c>
-      <c r="F21" s="50" t="str">
+      <c r="F21" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>19" Rounter Mount Kit</v>
       </c>
-      <c r="G21" s="49" t="str">
+      <c r="G21" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Mount Kit</v>
       </c>
-      <c r="H21" s="51">
+      <c r="H21" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>10</v>
       </c>
-      <c r="I21" s="52">
+      <c r="I21" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="C22" s="60" t="s">
+      <c r="C22" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="D22" s="62" t="s">
+      <c r="D22" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="E22" s="61">
+      <c r="E22" s="56">
         <v>3</v>
       </c>
-      <c r="F22" s="50" t="str">
+      <c r="F22" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>19"  Switch Rack Mount Kit</v>
       </c>
-      <c r="G22" s="49" t="str">
+      <c r="G22" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Mount Kit</v>
       </c>
-      <c r="H22" s="51">
+      <c r="H22" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>10</v>
       </c>
-      <c r="I22" s="52">
+      <c r="I22" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="C23" s="60" t="s">
+      <c r="C23" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="D23" s="62" t="s">
+      <c r="D23" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="E23" s="61">
+      <c r="E23" s="56">
         <v>1</v>
       </c>
-      <c r="F23" s="50" t="str">
+      <c r="F23" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>Cable Cove 2-Post Rack</v>
       </c>
-      <c r="G23" s="49" t="str">
+      <c r="G23" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Rack</v>
       </c>
-      <c r="H23" s="51">
+      <c r="H23" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>595</v>
       </c>
-      <c r="I23" s="52">
+      <c r="I23" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>595</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="48" t="s">
+      <c r="B24" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="60" t="s">
+      <c r="C24" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="D24" s="62" t="s">
+      <c r="D24" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="E24" s="61">
+      <c r="E24" s="56">
         <v>1</v>
       </c>
-      <c r="F24" s="50" t="str">
+      <c r="F24" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>Cisco 2951, SRE 700 SM, NME WAE 502, WAAS Ent, IOS Sec PAK</v>
       </c>
-      <c r="G24" s="49" t="str">
+      <c r="G24" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Router</v>
       </c>
-      <c r="H24" s="51">
+      <c r="H24" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>14995</v>
       </c>
-      <c r="I24" s="52">
+      <c r="I24" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>14995</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="60" t="s">
+      <c r="C25" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="62" t="s">
+      <c r="D25" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="E25" s="61">
+      <c r="E25" s="56">
         <v>6</v>
       </c>
-      <c r="F25" s="50" t="str">
+      <c r="F25" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>C9200-48T-E Catalyst 9200 Managed L3 Switch - 48 Ethernet Ports</v>
       </c>
-      <c r="G25" s="49" t="str">
+      <c r="G25" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Switch</v>
       </c>
-      <c r="H25" s="51">
+      <c r="H25" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>2665</v>
       </c>
-      <c r="I25" s="52">
+      <c r="I25" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>15990</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="60" t="s">
+      <c r="C26" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="62" t="s">
+      <c r="D26" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="61">
+      <c r="E26" s="56">
         <v>1</v>
       </c>
-      <c r="F26" s="50" t="str">
+      <c r="F26" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>19" Rounter Mount Kit</v>
       </c>
-      <c r="G26" s="49" t="str">
+      <c r="G26" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Mount Kit</v>
       </c>
-      <c r="H26" s="51">
+      <c r="H26" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>10</v>
       </c>
-      <c r="I26" s="52">
+      <c r="I26" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>10</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="48" t="s">
+      <c r="B27" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="62" t="s">
+      <c r="D27" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="E27" s="61">
+      <c r="E27" s="56">
         <v>6</v>
       </c>
-      <c r="F27" s="50" t="str">
+      <c r="F27" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>19"  Switch Rack Mount Kit</v>
       </c>
-      <c r="G27" s="49" t="str">
+      <c r="G27" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Mount Kit</v>
       </c>
-      <c r="H27" s="51">
+      <c r="H27" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>10</v>
       </c>
-      <c r="I27" s="52">
+      <c r="I27" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>60</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B28" s="48" t="s">
+      <c r="B28" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="C28" s="60" t="s">
+      <c r="C28" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="62" t="s">
+      <c r="D28" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="E28" s="61">
+      <c r="E28" s="56">
         <v>1</v>
       </c>
-      <c r="F28" s="50" t="str">
+      <c r="F28" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>Cable Cove 2-Post Rack</v>
       </c>
-      <c r="G28" s="49" t="str">
+      <c r="G28" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Rack</v>
       </c>
-      <c r="H28" s="51">
+      <c r="H28" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>595</v>
       </c>
-      <c r="I28" s="52">
+      <c r="I28" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>595</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="D29" s="62" t="s">
+      <c r="D29" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="E29" s="61">
+      <c r="E29" s="56">
         <v>1</v>
       </c>
-      <c r="F29" s="50" t="str">
+      <c r="F29" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>Cisco 2951, SRE 700 SM, NME WAE 502, WAAS Ent, IOS Sec PAK</v>
       </c>
-      <c r="G29" s="49" t="str">
+      <c r="G29" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Router</v>
       </c>
-      <c r="H29" s="51">
+      <c r="H29" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>14995</v>
       </c>
-      <c r="I29" s="52">
+      <c r="I29" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>14995</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B30" s="48" t="s">
+      <c r="B30" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="60" t="s">
+      <c r="C30" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="D30" s="62" t="s">
+      <c r="D30" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="E30" s="61">
+      <c r="E30" s="56">
         <v>8</v>
       </c>
-      <c r="F30" s="50" t="str">
+      <c r="F30" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>C9200-48T-E Catalyst 9200 Managed L3 Switch - 48 Ethernet Ports</v>
       </c>
-      <c r="G30" s="49" t="str">
+      <c r="G30" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Switch</v>
       </c>
-      <c r="H30" s="51">
+      <c r="H30" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>2665</v>
       </c>
-      <c r="I30" s="52">
+      <c r="I30" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>21320</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="C31" s="60" t="s">
+      <c r="C31" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="62" t="s">
+      <c r="D31" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="E31" s="61">
+      <c r="E31" s="56">
         <v>1</v>
       </c>
-      <c r="F31" s="50" t="str">
+      <c r="F31" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>19" Rounter Mount Kit</v>
       </c>
-      <c r="G31" s="49" t="str">
+      <c r="G31" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Mount Kit</v>
       </c>
-      <c r="H31" s="51">
+      <c r="H31" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>10</v>
       </c>
-      <c r="I31" s="52">
+      <c r="I31" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>10</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B32" s="48" t="s">
+      <c r="B32" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="C32" s="60" t="s">
+      <c r="C32" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="D32" s="62" t="s">
+      <c r="D32" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="E32" s="61">
+      <c r="E32" s="56">
         <v>8</v>
       </c>
-      <c r="F32" s="50" t="str">
+      <c r="F32" s="48" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>19"  Switch Rack Mount Kit</v>
       </c>
-      <c r="G32" s="49" t="str">
+      <c r="G32" s="47" t="str">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>Mount Kit</v>
       </c>
-      <c r="H32" s="51">
+      <c r="H32" s="49">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v>10</v>
       </c>
-      <c r="I32" s="52">
+      <c r="I32" s="50">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v>80</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="48"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="50">
+      <c r="B33" s="46"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="48">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>0</v>
       </c>
-      <c r="G33" s="49">
+      <c r="G33" s="47">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>0</v>
       </c>
-      <c r="H33" s="51" t="str">
+      <c r="H33" s="49" t="str">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I33" s="52" t="str">
+      <c r="I33" s="50" t="str">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="48"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="50">
+      <c r="B34" s="46"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="48">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>0</v>
       </c>
-      <c r="G34" s="49">
+      <c r="G34" s="47">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>0</v>
       </c>
-      <c r="H34" s="51" t="str">
+      <c r="H34" s="49" t="str">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I34" s="52" t="str">
+      <c r="I34" s="50" t="str">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B35" s="48"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="50">
+      <c r="B35" s="46"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="48">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>0</v>
       </c>
-      <c r="G35" s="49">
+      <c r="G35" s="47">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>0</v>
       </c>
-      <c r="H35" s="51" t="str">
+      <c r="H35" s="49" t="str">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I35" s="52" t="str">
+      <c r="I35" s="50" t="str">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B36" s="48"/>
-      <c r="C36" s="60"/>
-      <c r="D36" s="62"/>
-      <c r="E36" s="61"/>
-      <c r="F36" s="50">
+      <c r="B36" s="46"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="48">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="49">
+      <c r="G36" s="47">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>0</v>
       </c>
-      <c r="H36" s="51" t="str">
+      <c r="H36" s="49" t="str">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I36" s="52" t="str">
+      <c r="I36" s="50" t="str">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B37" s="48"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="61"/>
-      <c r="F37" s="50">
+      <c r="B37" s="46"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="48">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="49">
+      <c r="G37" s="47">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="51" t="str">
+      <c r="H37" s="49" t="str">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I37" s="52" t="str">
+      <c r="I37" s="50" t="str">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B38" s="48"/>
-      <c r="C38" s="60"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="61"/>
-      <c r="F38" s="50">
+      <c r="B38" s="46"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="48">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>0</v>
       </c>
-      <c r="G38" s="49">
+      <c r="G38" s="47">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>0</v>
       </c>
-      <c r="H38" s="51" t="str">
+      <c r="H38" s="49" t="str">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I38" s="52" t="str">
+      <c r="I38" s="50" t="str">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B39" s="48"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="62"/>
-      <c r="E39" s="61"/>
-      <c r="F39" s="50">
+      <c r="B39" s="46"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="56"/>
+      <c r="F39" s="48">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>0</v>
       </c>
-      <c r="G39" s="49">
+      <c r="G39" s="47">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>0</v>
       </c>
-      <c r="H39" s="51" t="str">
+      <c r="H39" s="49" t="str">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I39" s="52" t="str">
+      <c r="I39" s="50" t="str">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B40" s="48"/>
-      <c r="C40" s="60"/>
-      <c r="D40" s="62"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="50">
+      <c r="B40" s="46"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="56"/>
+      <c r="F40" s="48">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>0</v>
       </c>
-      <c r="G40" s="49">
+      <c r="G40" s="47">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>0</v>
       </c>
-      <c r="H40" s="51" t="str">
+      <c r="H40" s="49" t="str">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I40" s="52" t="str">
+      <c r="I40" s="50" t="str">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B41" s="48"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="50">
+      <c r="B41" s="46"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="48">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>0</v>
       </c>
-      <c r="G41" s="49">
+      <c r="G41" s="47">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>0</v>
       </c>
-      <c r="H41" s="51" t="str">
+      <c r="H41" s="49" t="str">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I41" s="52" t="str">
+      <c r="I41" s="50" t="str">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B42" s="48"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="50">
+      <c r="B42" s="46"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="48">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>0</v>
       </c>
-      <c r="G42" s="49">
+      <c r="G42" s="47">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>0</v>
       </c>
-      <c r="H42" s="51" t="str">
+      <c r="H42" s="49" t="str">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I42" s="52" t="str">
+      <c r="I42" s="50" t="str">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B43" s="58"/>
-      <c r="C43" s="60"/>
-      <c r="D43" s="62"/>
-      <c r="E43" s="61"/>
-      <c r="F43" s="57">
+      <c r="B43" s="54"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="56"/>
+      <c r="F43" s="48">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!D:D,"",0)</f>
         <v>0</v>
       </c>
-      <c r="G43" s="59">
+      <c r="G43" s="47">
         <f>_xlfn.XLOOKUP(Table2[[#This Row],[Item]],'Price List'!A:A,'Price List'!C:C,"",0)</f>
         <v>0</v>
       </c>
-      <c r="H43" s="51" t="str">
+      <c r="H43" s="49" t="str">
         <f>IFERROR(VLOOKUP(Table2[[#This Row],[Item]],parts[],H$10,FALSE),"")</f>
         <v/>
       </c>
-      <c r="I43" s="52" t="str">
+      <c r="I43" s="50" t="str">
         <f>IFERROR(Table2[[#This Row],[Qty]]*Table2[[#This Row],[Retail Price]],"")</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="34" t="s">
         <v>10</v>
       </c>
       <c r="H44" s="13"/>
-      <c r="I44" s="36">
+      <c r="I44" s="35">
         <f>SUBTOTAL(109,Table2[Cost])</f>
         <v>123925</v>
       </c>
     </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B45" s="34"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="35"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" s="34"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="35"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B47" s="34"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="35"/>
+    </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="H48" s="56" t="s">
+      <c r="B48" s="34"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="35"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B49" s="34"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="35"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B50" s="34"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="35"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B51" s="34"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="35"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B52" s="34"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="35"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B53" s="34"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="35"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H57" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="I48" s="56"/>
-    </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="I49" s="13"/>
-    </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="H50" s="37" t="s">
+      <c r="I57" s="60"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I58" s="13"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H59" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="I50" s="37" t="s">
+      <c r="I59" s="36" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="H51" s="63" t="s">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H60" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="I51" s="15">
-        <f>SUMIF(Table2[Installation Location],H51,Table2[Cost])</f>
+      <c r="I60" s="15">
+        <f>SUMIF(Table2[Installation Location],H60,Table2[Cost])</f>
         <v>31650</v>
       </c>
     </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="H52" s="15" t="s">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H61" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="I52" s="15">
-        <f>SUMIF(Table2[Cost],H52,Table2[Installation Location])</f>
+      <c r="I61" s="15">
+        <f>SUMIF(Table2[Cost],H61,Table2[Installation Location])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="H53" s="15" t="s">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H62" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="I53" s="15">
-        <f>SUMIF(Table2[Cost],H53,Table2[Installation Location])</f>
+      <c r="I62" s="15">
+        <f>SUMIF(Table2[Cost],H62,Table2[Installation Location])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="H54" s="15" t="s">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="H63" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="I54" s="15">
-        <f>SUMIF(Table2[Cost],H54,Table2[Installation Location])</f>
+      <c r="I63" s="15">
+        <f>SUMIF(Table2[Cost],H63,Table2[Installation Location])</f>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.2">
-      <c r="I55" s="15">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="I64" s="15">
         <f>SUMIFS(Table2[Cost],Table2[Installation Location],#REF!)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H56" s="53"/>
-      <c r="I56" s="53">
-        <f>SUM(I51:I55)</f>
+    <row r="65" spans="8:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H65" s="51"/>
+      <c r="I65" s="51">
+        <f>SUM(I60:I64)</f>
         <v>31650</v>
       </c>
     </row>
-    <row r="57" spans="8:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="66" spans="8:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H57:I57"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <dataValidations count="2">
@@ -3235,7 +3249,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="73" orientation="portrait" horizontalDpi="75" verticalDpi="75" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="75" verticalDpi="75" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;P&amp;CNetTRON&amp;R&amp;D</oddHeader>
   </headerFooter>
@@ -3249,7 +3263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>

</xml_diff>